<commit_message>
Split ISIC codes in 9 more variables (#89)
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoDSCbRIC/Shr of Dist Solar Costs by Rcpnt ISIC Code.xlsx
+++ b/InputData/bldgs/SoDSCbRIC/Shr of Dist Solar Costs by Rcpnt ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\bldgs\SoDSCbRIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0318BFB-A884-40BE-884D-423319545896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE39E34D-69A6-4F3D-B443-E81143DC1E93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="435" windowWidth="26295" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="105" windowWidth="25665" windowHeight="16830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
   <si>
     <t>https://www.nrel.gov/docs/fy19osti/72399.pdf</t>
   </si>
@@ -139,12 +139,6 @@
     <t>Rubber and plastics products</t>
   </si>
   <si>
-    <t>Other non-metallic mineral products</t>
-  </si>
-  <si>
-    <t>Manufacture of basic metals</t>
-  </si>
-  <si>
     <t>Fabricated metal products, except machinery and equipment</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
     <t>Other manufacturing; repair and installation of machinery and equipment</t>
   </si>
   <si>
-    <t>Electricity, gas, water supply, sewerage, waste and remediation services</t>
-  </si>
-  <si>
     <t>Construction</t>
   </si>
   <si>
@@ -244,12 +235,6 @@
     <t>ISIC 22</t>
   </si>
   <si>
-    <t>ISIC 23</t>
-  </si>
-  <si>
-    <t>ISIC 24</t>
-  </si>
-  <si>
     <t>ISIC 25</t>
   </si>
   <si>
@@ -271,9 +256,6 @@
     <t>ISIC 31T33</t>
   </si>
   <si>
-    <t>ISIC 35T39</t>
-  </si>
-  <si>
     <t>ISIC 41T43</t>
   </si>
   <si>
@@ -383,6 +365,48 @@
   </si>
   <si>
     <t>Oil and gas extraction</t>
+  </si>
+  <si>
+    <t>ISIC 231</t>
+  </si>
+  <si>
+    <t>ISIC 239</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>Cement and other nonmetallic minerals</t>
+  </si>
+  <si>
+    <t>ISIC 241</t>
+  </si>
+  <si>
+    <t>ISIC 242</t>
+  </si>
+  <si>
+    <t>Iron and steel</t>
+  </si>
+  <si>
+    <t>Other metals</t>
+  </si>
+  <si>
+    <t>ISIC 351</t>
+  </si>
+  <si>
+    <t>ISIC 352T353</t>
+  </si>
+  <si>
+    <t>ISIC 36T39</t>
+  </si>
+  <si>
+    <t>Electricity generation and distribution</t>
+  </si>
+  <si>
+    <t>Energy pipelines and gas processing</t>
+  </si>
+  <si>
+    <t>Water and waste</t>
   </si>
 </sst>
 </file>
@@ -763,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -772,15 +796,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +814,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,27 +824,27 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +858,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -860,7 +884,7 @@
         <v>24</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -868,19 +892,19 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -902,13 +926,13 @@
         <v>0.11115462948456839</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -927,13 +951,13 @@
         <v>0.10778630737897542</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,10 +976,10 @@
         <v>0.11789127369575435</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -977,10 +1001,10 @@
         <v>2.020993263355789E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
         <v>27</v>
@@ -1002,10 +1026,10 @@
         <v>9.0944696851010504E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
         <v>28</v>
@@ -1026,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
         <v>29</v>
@@ -1048,10 +1072,10 @@
         <v>0.12454958483471723</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -1073,10 +1097,10 @@
         <v>9.4234685884380387E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -1098,10 +1122,10 @@
         <v>5.7183142722857593E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
         <v>32</v>
@@ -1123,13 +1147,13 @@
         <v>9.4234685884380387E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1148,18 +1172,18 @@
         <v>0.1818110606297979</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -1174,10 +1198,10 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1185,22 +1209,22 @@
         <v>22</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1219,13 +1243,13 @@
         <v>5.9203313436472164E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,13 +1268,13 @@
         <v>2.4668047265196738E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="H18" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1269,13 +1293,13 @@
         <v>0.17760994030941649</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1293,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,13 +1339,13 @@
         <v>4.9336094530393476E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1340,13 +1364,13 @@
         <v>8.8804970154708243E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,13 +1389,13 @@
         <v>7.8937751248629548E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1390,13 +1414,13 @@
         <v>9.9524911682299919E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1415,13 +1439,13 @@
         <v>8.9657692776221209E-2</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1440,13 +1464,13 @@
         <v>6.9923254964063833E-2</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="H26" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1465,109 +1489,141 @@
         <v>0.26233402363259839</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="H28" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H30" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H31" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H34" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H35" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="H37" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H38" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="H39" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>86</v>
+      </c>
+      <c r="H42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1580,134 +1636,146 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AM4"/>
+  <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="L1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="O1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="N1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="AD1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AK1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AL1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AM1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AN1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AO1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AP1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AQ1" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>87</v>
-      </c>
-      <c r="AH1" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ1" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM1" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>93</v>
       </c>
       <c r="B2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!B1,Data!$D$3:$D$13)</f>
@@ -1771,23 +1839,23 @@
       </c>
       <c r="Q2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!Q1,Data!$D$3:$D$13)</f>
-        <v>5.7183142722857593E-2</v>
+        <v>0</v>
       </c>
       <c r="R2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!R1,Data!$D$3:$D$13)</f>
-        <v>0.1818110606297979</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!S1,Data!$D$3:$D$13)</f>
-        <v>0.18846937176876077</v>
+        <v>5.7183142722857593E-2</v>
       </c>
       <c r="T2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!T1,Data!$D$3:$D$13)</f>
-        <v>0</v>
+        <v>0.1818110606297979</v>
       </c>
       <c r="U2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!U1,Data!$D$3:$D$13)</f>
-        <v>0</v>
+        <v>0.18846937176876077</v>
       </c>
       <c r="V2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!V1,Data!$D$3:$D$13)</f>
@@ -1803,7 +1871,7 @@
       </c>
       <c r="Y2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!Y1,Data!$D$3:$D$13)</f>
-        <v>0.30988563371455435</v>
+        <v>0</v>
       </c>
       <c r="Z2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!Z1,Data!$D$3:$D$13)</f>
@@ -1811,7 +1879,7 @@
       </c>
       <c r="AA2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AA1,Data!$D$3:$D$13)</f>
-        <v>0.12454958483471723</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AB1,Data!$D$3:$D$13)</f>
@@ -1819,7 +1887,7 @@
       </c>
       <c r="AC2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AC1,Data!$D$3:$D$13)</f>
-        <v>0</v>
+        <v>0.30988563371455435</v>
       </c>
       <c r="AD2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AD1,Data!$D$3:$D$13)</f>
@@ -1827,7 +1895,7 @@
       </c>
       <c r="AE2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AE1,Data!$D$3:$D$13)</f>
-        <v>0</v>
+        <v>0.12454958483471723</v>
       </c>
       <c r="AF2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AF1,Data!$D$3:$D$13)</f>
@@ -1839,7 +1907,7 @@
       </c>
       <c r="AH2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AH1,Data!$D$3:$D$13)</f>
-        <v>0.13810120632931225</v>
+        <v>0</v>
       </c>
       <c r="AI2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AI1,Data!$D$3:$D$13)</f>
@@ -1855,23 +1923,39 @@
       </c>
       <c r="AL2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AL1,Data!$D$3:$D$13)</f>
-        <v>0</v>
+        <v>0.13810120632931225</v>
       </c>
       <c r="AM2">
         <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AM1,Data!$D$3:$D$13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN2">
+        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AN1,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AO1,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AP1,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AQ1,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B3">
         <f>B2</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:AM3" si="0">C2</f>
+        <f t="shared" ref="C3:AQ3" si="0">C2</f>
         <v>0</v>
       </c>
       <c r="D3">
@@ -1923,29 +2007,29 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="P3" si="3">P2</f>
         <v>0</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3" si="4">R2</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
         <v>5.7183142722857593E-2</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <f t="shared" si="0"/>
         <v>0.1818110606297979</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <f t="shared" si="0"/>
         <v>0.18846937176876077</v>
       </c>
-      <c r="T3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="V3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1960,32 +2044,32 @@
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AB3" si="5">AA2</f>
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" si="0"/>
         <v>0.30988563371455435</v>
       </c>
-      <c r="Z3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA3">
+      <c r="AD3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE3">
         <f t="shared" si="0"/>
         <v>0.12454958483471723</v>
       </c>
-      <c r="AB3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AF3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1996,32 +2080,48 @@
       </c>
       <c r="AH3">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" si="0"/>
         <v>0.13810120632931225</v>
       </c>
-      <c r="AI3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AM3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!B1,Data!$D$17:$D$27)</f>
@@ -2085,23 +2185,23 @@
       </c>
       <c r="Q4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!Q1,Data!$D$17:$D$27)</f>
-        <v>8.9657692776221209E-2</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!R1,Data!$D$17:$D$27)</f>
-        <v>0.26233402363259839</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!S1,Data!$D$17:$D$27)</f>
-        <v>0.16944816664636375</v>
+        <v>8.9657692776221209E-2</v>
       </c>
       <c r="T4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!T1,Data!$D$17:$D$27)</f>
-        <v>0</v>
+        <v>0.26233402363259839</v>
       </c>
       <c r="U4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!U1,Data!$D$17:$D$27)</f>
-        <v>0</v>
+        <v>0.16944816664636375</v>
       </c>
       <c r="V4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!V1,Data!$D$17:$D$27)</f>
@@ -2117,7 +2217,7 @@
       </c>
       <c r="Y4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!Y1,Data!$D$17:$D$27)</f>
-        <v>0.42922402241442315</v>
+        <v>0</v>
       </c>
       <c r="Z4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!Z1,Data!$D$17:$D$27)</f>
@@ -2133,7 +2233,7 @@
       </c>
       <c r="AC4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AC1,Data!$D$17:$D$27)</f>
-        <v>0</v>
+        <v>0.42922402241442315</v>
       </c>
       <c r="AD4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AD1,Data!$D$17:$D$27)</f>
@@ -2153,7 +2253,7 @@
       </c>
       <c r="AH4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AH1,Data!$D$17:$D$27)</f>
-        <v>4.9336094530393476E-2</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AI1,Data!$D$17:$D$27)</f>
@@ -2169,10 +2269,26 @@
       </c>
       <c r="AL4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AL1,Data!$D$17:$D$27)</f>
-        <v>0</v>
+        <v>4.9336094530393476E-2</v>
       </c>
       <c r="AM4">
         <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AM1,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AN1,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AO1,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AP1,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AQ1,Data!$D$17:$D$27)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>